<commit_message>
use analysis class with excel parsing
</commit_message>
<xml_diff>
--- a/spec/files/0_1_09_setup_version_2.xlsx
+++ b/spec/files/0_1_09_setup_version_2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="2800" windowWidth="22800" windowHeight="13260" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -3002,15 +3002,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1285">
@@ -4913,9 +4913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4955,14 +4955,14 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="28" t="s">
+      <c r="Q1" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
     </row>
     <row r="2" spans="1:22" s="9" customFormat="1" ht="15">
       <c r="A2" s="9" t="s">
@@ -5780,7 +5780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:G3"/>
     </sheetView>
@@ -5822,50 +5822,50 @@
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
     </row>
     <row r="2" spans="1:22" s="9" customFormat="1" ht="15">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>492</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>493</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>494</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>495</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>496</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="28" t="s">
         <v>499</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>500</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:22" s="16" customFormat="1" ht="30">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29" t="s">
         <v>497</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="29" t="s">
         <v>498</v>
       </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="30" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="29" t="s">
         <v>501</v>
       </c>
       <c r="H3" s="11"/>

</xml_diff>